<commit_message>
Analysis + Data visualisation
</commit_message>
<xml_diff>
--- a/data/adult_fly_weight.xlsx
+++ b/data/adult_fly_weight.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40c2179675f51a02/Amy Butler Research Project/Medfly-Development-Study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79ED013E-F74E-4E95-B293-18EE28CB68C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{79ED013E-F74E-4E95-B293-18EE28CB68C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B219A741-3457-4A49-AD65-E3B81016132F}"/>
   <bookViews>
-    <workbookView xWindow="-10241" yWindow="518" windowWidth="16589" windowHeight="8663" xr2:uid="{5D4C8983-B229-4D54-90B2-8A009013FAF3}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="16589" windowHeight="8663" xr2:uid="{5D4C8983-B229-4D54-90B2-8A009013FAF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>parental_egg_collection_date</t>
   </si>
   <si>
-    <t>pupae_diet</t>
-  </si>
-  <si>
     <t>S2</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>weight (mg)</t>
+  </si>
+  <si>
+    <t>larval_diet</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED1975B-A257-4877-941D-B04A3FA26979}">
   <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -452,24 +454,24 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>44608</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>2.63</v>
@@ -477,16 +479,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>44608</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>3.3359999999999999</v>
@@ -494,16 +496,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>44608</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>2.8980000000000001</v>
@@ -511,16 +513,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>44608</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>3.4580000000000002</v>
@@ -528,16 +530,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>44608</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>3.3769999999999998</v>
@@ -545,16 +547,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>44608</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>2.82</v>
@@ -562,16 +564,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>44608</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>2.3820000000000001</v>
@@ -579,16 +581,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>44608</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>2.8860000000000001</v>
@@ -596,16 +598,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1">
         <v>44608</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>2.72</v>
@@ -613,16 +615,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
         <v>44608</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>2.9009999999999998</v>
@@ -630,16 +632,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
         <v>44608</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12">
         <v>3.0790000000000002</v>
@@ -647,16 +649,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <v>44608</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <v>3.1709999999999998</v>
@@ -664,16 +666,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>44608</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14">
         <v>2.94</v>
@@ -681,16 +683,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
         <v>44608</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>3.0579999999999998</v>
@@ -698,16 +700,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1">
         <v>44608</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16">
         <v>2.58</v>
@@ -715,16 +717,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1">
         <v>44608</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>2.9289999999999998</v>
@@ -732,16 +734,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
         <v>44608</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <v>3.2679999999999998</v>
@@ -749,16 +751,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
         <v>44608</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19">
         <v>3.2450000000000001</v>
@@ -766,16 +768,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1">
         <v>44608</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20">
         <v>3.0529999999999999</v>
@@ -783,16 +785,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
         <v>44608</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <v>2.8580000000000001</v>
@@ -800,16 +802,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
         <v>44608</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>3.2130000000000001</v>
@@ -817,16 +819,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
         <v>44608</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>3.3919999999999999</v>
@@ -834,16 +836,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <v>44608</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24">
         <v>2.7610000000000001</v>
@@ -851,16 +853,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1">
         <v>44608</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25">
         <v>3.625</v>
@@ -868,16 +870,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1">
         <v>44608</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>2.99</v>
@@ -885,16 +887,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1">
         <v>44608</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27">
         <v>3.1429999999999998</v>
@@ -902,16 +904,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
         <v>44608</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28">
         <v>2.8660000000000001</v>
@@ -919,16 +921,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1">
         <v>44608</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29">
         <v>3.4319999999999999</v>
@@ -936,16 +938,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1">
         <v>44608</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30">
         <v>3.0920000000000001</v>
@@ -953,16 +955,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1">
         <v>44608</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31">
         <v>2.9049999999999998</v>
@@ -970,16 +972,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="1">
         <v>44608</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32">
         <v>3.677</v>
@@ -987,16 +989,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="1">
         <v>44608</v>
       </c>
       <c r="D33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33">
         <v>3.4020000000000001</v>
@@ -1004,16 +1006,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" s="1">
         <v>44608</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34">
         <v>3.972</v>
@@ -1021,16 +1023,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1">
         <v>44608</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35">
         <v>3.5230000000000001</v>
@@ -1038,16 +1040,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="1">
         <v>44608</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E36">
         <v>4.0990000000000002</v>
@@ -1055,16 +1057,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="1">
         <v>44608</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E37">
         <v>3.0979999999999999</v>
@@ -1072,16 +1074,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="1">
         <v>44608</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E38">
         <v>3.2749999999999999</v>
@@ -1089,16 +1091,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" s="1">
         <v>44608</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39">
         <v>3.2389999999999999</v>
@@ -1106,16 +1108,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="1">
         <v>44608</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40">
         <v>2.843</v>
@@ -1123,16 +1125,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41" s="1">
         <v>44608</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41">
         <v>3.3780000000000001</v>
@@ -1140,16 +1142,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42" s="1">
         <v>44608</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42">
         <v>3.6549999999999998</v>
@@ -1157,16 +1159,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" s="1">
         <v>44608</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E43">
         <v>3.5430000000000001</v>
@@ -1174,16 +1176,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" s="1">
         <v>44608</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44">
         <v>3.4249999999999998</v>
@@ -1191,16 +1193,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45" s="1">
         <v>44608</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E45">
         <v>3.117</v>
@@ -1208,16 +1210,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46" s="1">
         <v>44608</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E46">
         <v>3.2349999999999999</v>
@@ -1225,16 +1227,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47" s="1">
         <v>44608</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E47">
         <v>3.37</v>
@@ -1242,16 +1244,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="1">
         <v>44608</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E48">
         <v>2.6339999999999999</v>
@@ -1259,16 +1261,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" s="1">
         <v>44608</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49">
         <v>2.9969999999999999</v>
@@ -1276,16 +1278,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1">
         <v>44608</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E50">
         <v>3.161</v>
@@ -1293,16 +1295,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C51" s="1">
         <v>44608</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E51">
         <v>3.1419999999999999</v>
@@ -1310,16 +1312,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C52" s="1">
         <v>44608</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52">
         <v>3.343</v>
@@ -1327,16 +1329,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" s="1">
         <v>44608</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E53">
         <v>3.3460000000000001</v>
@@ -1344,16 +1346,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1">
         <v>44608</v>
       </c>
       <c r="D54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E54">
         <v>3.3889999999999998</v>
@@ -1361,16 +1363,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55" s="1">
         <v>44608</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E55">
         <v>3.3940000000000001</v>
@@ -1378,16 +1380,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="1">
         <v>44608</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E56">
         <v>3.464</v>
@@ -1395,16 +1397,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57" s="1">
         <v>44609</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57">
         <v>2.8090000000000002</v>
@@ -1412,16 +1414,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58" s="1">
         <v>44609</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E58">
         <v>3.2610000000000001</v>
@@ -1429,16 +1431,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C59" s="1">
         <v>44609</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E59">
         <v>2.7959999999999998</v>
@@ -1446,16 +1448,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60" s="1">
         <v>44609</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E60">
         <v>3.6219999999999999</v>
@@ -1463,16 +1465,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61" s="1">
         <v>44609</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E61">
         <v>2.6920000000000002</v>
@@ -1480,16 +1482,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62" s="1">
         <v>44609</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E62">
         <v>3.42</v>
@@ -1497,16 +1499,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63" s="1">
         <v>44609</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E63">
         <v>2.8530000000000002</v>
@@ -1514,16 +1516,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64" s="1">
         <v>44609</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E64">
         <v>3.1309999999999998</v>
@@ -1531,16 +1533,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" s="1">
         <v>44609</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E65">
         <v>2.7989999999999999</v>
@@ -1548,16 +1550,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66" s="1">
         <v>44609</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E66">
         <v>2.6520000000000001</v>
@@ -1565,16 +1567,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67" s="1">
         <v>44609</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E67">
         <v>3.3479999999999999</v>
@@ -1582,16 +1584,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68" s="1">
         <v>44609</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E68">
         <v>2.859</v>
@@ -1599,16 +1601,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" s="1">
         <v>44609</v>
       </c>
       <c r="D69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E69">
         <v>3.2879999999999998</v>
@@ -1616,16 +1618,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70" s="1">
         <v>44609</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E70">
         <v>2.8279999999999998</v>
@@ -1633,16 +1635,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" s="1">
         <v>44609</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E71">
         <v>3.4180000000000001</v>
@@ -1650,16 +1652,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C72" s="1">
         <v>44609</v>
       </c>
       <c r="D72" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E72">
         <v>2.6259999999999999</v>
@@ -1667,16 +1669,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C73" s="1">
         <v>44609</v>
       </c>
       <c r="D73" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E73">
         <v>2.8140000000000001</v>
@@ -1684,16 +1686,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C74" s="1">
         <v>44609</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E74">
         <v>2.9660000000000002</v>
@@ -1701,16 +1703,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75" s="1">
         <v>44609</v>
       </c>
       <c r="D75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E75">
         <v>3.3279999999999998</v>
@@ -1718,16 +1720,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76" s="1">
         <v>44609</v>
       </c>
       <c r="D76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E76">
         <v>2.93</v>
@@ -1735,16 +1737,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77" s="1">
         <v>44609</v>
       </c>
       <c r="D77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E77">
         <v>3.351</v>
@@ -1752,16 +1754,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C78" s="1">
         <v>44609</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E78">
         <v>2.7639999999999998</v>
@@ -1769,16 +1771,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C79" s="1">
         <v>44609</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E79">
         <v>3.3159999999999998</v>
@@ -1786,16 +1788,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C80" s="1">
         <v>44609</v>
       </c>
       <c r="D80" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E80">
         <v>3.327</v>
@@ -1803,16 +1805,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C81" s="1">
         <v>44609</v>
       </c>
       <c r="D81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E81">
         <v>3.3260000000000001</v>
@@ -1820,16 +1822,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82" s="1">
         <v>44609</v>
       </c>
       <c r="D82" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E82">
         <v>3.24</v>
@@ -1837,16 +1839,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83" s="1">
         <v>44609</v>
       </c>
       <c r="D83" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E83">
         <v>2.944</v>
@@ -1854,16 +1856,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C84" s="1">
         <v>44609</v>
       </c>
       <c r="D84" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E84">
         <v>3.823</v>
@@ -1871,16 +1873,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C85" s="1">
         <v>44609</v>
       </c>
       <c r="D85" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E85">
         <v>3.1110000000000002</v>
@@ -1888,16 +1890,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C86" s="1">
         <v>44609</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E86">
         <v>2.6379999999999999</v>
@@ -1905,16 +1907,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C87" s="1">
         <v>44609</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E87">
         <v>3.8069999999999999</v>
@@ -1922,16 +1924,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C88" s="1">
         <v>44609</v>
       </c>
       <c r="D88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E88">
         <v>3.032</v>
@@ -1939,16 +1941,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C89" s="1">
         <v>44609</v>
       </c>
       <c r="D89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89">
         <v>3.4870000000000001</v>
@@ -1956,16 +1958,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C90" s="1">
         <v>44609</v>
       </c>
       <c r="D90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E90">
         <v>2.7839999999999998</v>
@@ -1973,16 +1975,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C91" s="1">
         <v>44609</v>
       </c>
       <c r="D91" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E91">
         <v>3.2970000000000002</v>
@@ -1990,16 +1992,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C92" s="1">
         <v>44609</v>
       </c>
       <c r="D92" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E92">
         <v>3.8069999999999999</v>
@@ -2007,16 +2009,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C93" s="1">
         <v>44609</v>
       </c>
       <c r="D93" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E93">
         <v>3.5449999999999999</v>
@@ -2024,16 +2026,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94" s="1">
         <v>44609</v>
       </c>
       <c r="D94" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E94">
         <v>3.2679999999999998</v>
@@ -2041,16 +2043,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C95" s="1">
         <v>44609</v>
       </c>
       <c r="D95" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E95">
         <v>3.8439999999999999</v>
@@ -2058,16 +2060,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C96" s="1">
         <v>44609</v>
       </c>
       <c r="D96" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E96">
         <v>4.1130000000000004</v>
@@ -2075,16 +2077,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C97" s="1">
         <v>44609</v>
       </c>
       <c r="D97" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E97">
         <v>2.6890000000000001</v>
@@ -2092,16 +2094,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C98" s="1">
         <v>44609</v>
       </c>
       <c r="D98" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E98">
         <v>3.5529999999999999</v>
@@ -2109,16 +2111,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C99" s="1">
         <v>44609</v>
       </c>
       <c r="D99" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E99">
         <v>2.9630000000000001</v>
@@ -2126,16 +2128,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C100" s="1">
         <v>44609</v>
       </c>
       <c r="D100" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E100">
         <v>2.472</v>
@@ -2143,16 +2145,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B101" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C101" s="1">
         <v>44609</v>
       </c>
       <c r="D101" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E101">
         <v>2.9660000000000002</v>
@@ -2160,16 +2162,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C102" s="1">
         <v>44609</v>
       </c>
       <c r="D102" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E102">
         <v>3.3359999999999999</v>
@@ -2177,16 +2179,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C103" s="1">
         <v>44609</v>
       </c>
       <c r="D103" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E103">
         <v>3.5329999999999999</v>
@@ -2194,16 +2196,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B104" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C104" s="1">
         <v>44609</v>
       </c>
       <c r="D104" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E104">
         <v>3.43</v>
@@ -2211,16 +2213,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B105" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C105" s="1">
         <v>44609</v>
       </c>
       <c r="D105" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E105">
         <v>3.2069999999999999</v>
@@ -2228,16 +2230,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B106" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C106" s="1">
         <v>44609</v>
       </c>
       <c r="D106" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E106">
         <v>3.3740000000000001</v>
@@ -2245,16 +2247,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C107" s="1">
         <v>44609</v>
       </c>
       <c r="D107" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E107">
         <v>2.859</v>
@@ -2262,16 +2264,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B108" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C108" s="1">
         <v>44609</v>
       </c>
       <c r="D108" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E108">
         <v>2.948</v>
@@ -2279,16 +2281,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C109" s="1">
         <v>44609</v>
       </c>
       <c r="D109" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E109">
         <v>3.472</v>
@@ -2296,16 +2298,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B110" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C110" s="1">
         <v>44609</v>
       </c>
       <c r="D110" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E110">
         <v>3.464</v>
@@ -2313,16 +2315,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C111" s="1">
         <v>44609</v>
       </c>
       <c r="D111" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E111">
         <v>3.2189999999999999</v>
@@ -2330,16 +2332,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B112" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C112" s="1">
         <v>44609</v>
       </c>
       <c r="D112" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E112">
         <v>3.2429999999999999</v>
@@ -2347,16 +2349,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C113" s="1">
         <v>44609</v>
       </c>
       <c r="D113" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E113">
         <v>3.7559999999999998</v>
@@ -2364,16 +2366,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B114" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C114" s="1">
         <v>44609</v>
       </c>
       <c r="D114" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E114">
         <v>3.3490000000000002</v>
@@ -2381,16 +2383,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B115" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C115" s="1">
         <v>44609</v>
       </c>
       <c r="D115" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E115">
         <v>3.3029999999999999</v>
@@ -2398,16 +2400,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B116" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C116" s="1">
         <v>44609</v>
       </c>
       <c r="D116" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E116">
         <v>3.2679999999999998</v>
@@ -2415,16 +2417,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C117" s="1">
         <v>44610</v>
       </c>
       <c r="D117" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E117">
         <v>2.7530000000000001</v>
@@ -2432,16 +2434,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B118" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C118" s="1">
         <v>44610</v>
       </c>
       <c r="D118" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E118">
         <v>3.4769999999999999</v>
@@ -2449,16 +2451,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C119" s="1">
         <v>44610</v>
       </c>
       <c r="D119" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E119">
         <v>3.0089999999999999</v>
@@ -2466,16 +2468,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B120" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C120" s="1">
         <v>44610</v>
       </c>
       <c r="D120" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E120">
         <v>3.371</v>
@@ -2483,16 +2485,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B121" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C121" s="1">
         <v>44610</v>
       </c>
       <c r="D121" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E121">
         <v>2.85</v>
@@ -2500,16 +2502,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B122" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C122" s="1">
         <v>44610</v>
       </c>
       <c r="D122" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E122">
         <v>3.4369999999999998</v>
@@ -2517,16 +2519,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B123" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C123" s="1">
         <v>44610</v>
       </c>
       <c r="D123" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E123">
         <v>3.12</v>
@@ -2534,16 +2536,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B124" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C124" s="1">
         <v>44610</v>
       </c>
       <c r="D124" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E124">
         <v>2.5390000000000001</v>
@@ -2551,16 +2553,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B125" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C125" s="1">
         <v>44610</v>
       </c>
       <c r="D125" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E125">
         <v>2.3679999999999999</v>
@@ -2568,16 +2570,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B126" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C126" s="1">
         <v>44610</v>
       </c>
       <c r="D126" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E126">
         <v>2.9039999999999999</v>
@@ -2585,16 +2587,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B127" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C127" s="1">
         <v>44610</v>
       </c>
       <c r="D127" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E127">
         <v>3.177</v>
@@ -2602,16 +2604,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B128" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C128" s="1">
         <v>44610</v>
       </c>
       <c r="D128" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E128">
         <v>2.484</v>
@@ -2619,16 +2621,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B129" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C129" s="1">
         <v>44610</v>
       </c>
       <c r="D129" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E129">
         <v>3.1469999999999998</v>
@@ -2636,16 +2638,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B130" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C130" s="1">
         <v>44610</v>
       </c>
       <c r="D130" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E130">
         <v>3.0289999999999999</v>
@@ -2653,16 +2655,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B131" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C131" s="1">
         <v>44610</v>
       </c>
       <c r="D131" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E131">
         <v>2.9140000000000001</v>
@@ -2670,16 +2672,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B132" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C132" s="1">
         <v>44610</v>
       </c>
       <c r="D132" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E132">
         <v>2.9809999999999999</v>
@@ -2687,16 +2689,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B133" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C133" s="1">
         <v>44610</v>
       </c>
       <c r="D133" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E133">
         <v>2.84</v>
@@ -2704,16 +2706,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B134" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C134" s="1">
         <v>44610</v>
       </c>
       <c r="D134" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E134">
         <v>2.7789999999999999</v>
@@ -2721,16 +2723,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B135" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C135" s="1">
         <v>44610</v>
       </c>
       <c r="D135" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E135">
         <v>2.9790000000000001</v>
@@ -2738,16 +2740,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B136" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C136" s="1">
         <v>44610</v>
       </c>
       <c r="D136" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E136">
         <v>2.9319999999999999</v>
@@ -2755,16 +2757,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B137" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C137" s="1">
         <v>44610</v>
       </c>
       <c r="D137" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E137">
         <v>2.8919999999999999</v>
@@ -2772,16 +2774,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C138" s="1">
         <v>44610</v>
       </c>
       <c r="D138" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E138">
         <v>3.4089999999999998</v>
@@ -2789,16 +2791,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B139" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C139" s="1">
         <v>44610</v>
       </c>
       <c r="D139" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E139">
         <v>3.351</v>
@@ -2806,16 +2808,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B140" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C140" s="1">
         <v>44610</v>
       </c>
       <c r="D140" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E140">
         <v>3.6339999999999999</v>
@@ -2823,16 +2825,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B141" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C141" s="1">
         <v>44610</v>
       </c>
       <c r="D141" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E141">
         <v>3.379</v>
@@ -2840,16 +2842,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B142" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C142" s="1">
         <v>44610</v>
       </c>
       <c r="D142" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E142">
         <v>3.1760000000000002</v>
@@ -2857,16 +2859,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B143" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C143" s="1">
         <v>44610</v>
       </c>
       <c r="D143" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E143">
         <v>3.1890000000000001</v>
@@ -2874,16 +2876,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B144" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C144" s="1">
         <v>44610</v>
       </c>
       <c r="D144" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E144">
         <v>3.202</v>
@@ -2891,16 +2893,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B145" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C145" s="1">
         <v>44610</v>
       </c>
       <c r="D145" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E145">
         <v>2.8279999999999998</v>
@@ -2908,16 +2910,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B146" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C146" s="1">
         <v>44610</v>
       </c>
       <c r="D146" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E146">
         <v>2.3570000000000002</v>
@@ -2925,16 +2927,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B147" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C147" s="1">
         <v>44610</v>
       </c>
       <c r="D147" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E147">
         <v>3.8140000000000001</v>
@@ -2942,16 +2944,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B148" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C148" s="1">
         <v>44610</v>
       </c>
       <c r="D148" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E148">
         <v>3.7909999999999999</v>
@@ -2959,16 +2961,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B149" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C149" s="1">
         <v>44610</v>
       </c>
       <c r="D149" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E149">
         <v>2.8439999999999999</v>
@@ -2976,16 +2978,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B150" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C150" s="1">
         <v>44610</v>
       </c>
       <c r="D150" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E150">
         <v>3.4809999999999999</v>
@@ -2993,16 +2995,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B151" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C151" s="1">
         <v>44610</v>
       </c>
       <c r="D151" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E151">
         <v>3.34</v>
@@ -3010,16 +3012,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B152" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C152" s="1">
         <v>44610</v>
       </c>
       <c r="D152" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E152">
         <v>3.7759999999999998</v>
@@ -3027,16 +3029,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B153" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C153" s="1">
         <v>44610</v>
       </c>
       <c r="D153" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E153">
         <v>3.3639999999999999</v>
@@ -3044,16 +3046,16 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B154" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C154" s="1">
         <v>44610</v>
       </c>
       <c r="D154" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E154">
         <v>3.448</v>
@@ -3061,16 +3063,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B155" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C155" s="1">
         <v>44610</v>
       </c>
       <c r="D155" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E155">
         <v>3.4319999999999999</v>
@@ -3078,16 +3080,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B156" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C156" s="1">
         <v>44610</v>
       </c>
       <c r="D156" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E156">
         <v>3.3889999999999998</v>
@@ -3095,16 +3097,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B157" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C157" s="1">
         <v>44610</v>
       </c>
       <c r="D157" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E157">
         <v>3.0190000000000001</v>
@@ -3112,16 +3114,16 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B158" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C158" s="1">
         <v>44610</v>
       </c>
       <c r="D158" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E158">
         <v>3.343</v>
@@ -3129,16 +3131,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B159" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C159" s="1">
         <v>44610</v>
       </c>
       <c r="D159" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E159">
         <v>2.9129999999999998</v>
@@ -3146,16 +3148,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B160" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C160" s="1">
         <v>44610</v>
       </c>
       <c r="D160" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E160">
         <v>3.4329999999999998</v>
@@ -3163,16 +3165,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B161" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C161" s="1">
         <v>44610</v>
       </c>
       <c r="D161" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E161">
         <v>3.3660000000000001</v>
@@ -3180,16 +3182,16 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B162" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C162" s="1">
         <v>44610</v>
       </c>
       <c r="D162" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E162">
         <v>3.351</v>
@@ -3197,16 +3199,16 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B163" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C163" s="1">
         <v>44610</v>
       </c>
       <c r="D163" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E163">
         <v>3.7240000000000002</v>
@@ -3214,16 +3216,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B164" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C164" s="1">
         <v>44610</v>
       </c>
       <c r="D164" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E164">
         <v>3.286</v>
@@ -3231,16 +3233,16 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B165" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C165" s="1">
         <v>44610</v>
       </c>
       <c r="D165" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E165">
         <v>3.1859999999999999</v>
@@ -3248,16 +3250,16 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B166" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C166" s="1">
         <v>44610</v>
       </c>
       <c r="D166" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E166">
         <v>3.0880000000000001</v>
@@ -3265,16 +3267,16 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B167" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C167" s="1">
         <v>44610</v>
       </c>
       <c r="D167" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E167">
         <v>3.016</v>
@@ -3282,16 +3284,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B168" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C168" s="1">
         <v>44610</v>
       </c>
       <c r="D168" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E168">
         <v>2.6640000000000001</v>
@@ -3299,16 +3301,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B169" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C169" s="1">
         <v>44610</v>
       </c>
       <c r="D169" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E169">
         <v>2.8769999999999998</v>
@@ -3316,16 +3318,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B170" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C170" s="1">
         <v>44610</v>
       </c>
       <c r="D170" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E170">
         <v>3.4009999999999998</v>
@@ -3333,16 +3335,16 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B171" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C171" s="1">
         <v>44610</v>
       </c>
       <c r="D171" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E171">
         <v>3.0920000000000001</v>
@@ -3350,16 +3352,16 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B172" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C172" s="1">
         <v>44610</v>
       </c>
       <c r="D172" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E172">
         <v>3.1850000000000001</v>
@@ -3367,16 +3369,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B173" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C173" s="1">
         <v>44610</v>
       </c>
       <c r="D173" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E173">
         <v>3.1989999999999998</v>
@@ -3384,16 +3386,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B174" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C174" s="1">
         <v>44610</v>
       </c>
       <c r="D174" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E174">
         <v>3.64</v>
@@ -3401,16 +3403,16 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B175" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C175" s="1">
         <v>44610</v>
       </c>
       <c r="D175" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E175">
         <v>3.3929999999999998</v>
@@ -3418,16 +3420,16 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B176" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C176" s="1">
         <v>44610</v>
       </c>
       <c r="D176" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E176">
         <v>3.351</v>

</xml_diff>

<commit_message>
Added Dissertation Script cleaning
</commit_message>
<xml_diff>
--- a/data/adult_fly_weight.xlsx
+++ b/data/adult_fly_weight.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{79ED013E-F74E-4E95-B293-18EE28CB68C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B219A741-3457-4A49-AD65-E3B81016132F}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="16589" windowHeight="8663" xr2:uid="{5D4C8983-B229-4D54-90B2-8A009013FAF3}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12165" xr2:uid="{5D4C8983-B229-4D54-90B2-8A009013FAF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:E176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>